<commit_message>
Prototypy imprezy i skladnikow
</commit_message>
<xml_diff>
--- a/historie.xlsx
+++ b/historie.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="70">
   <si>
     <t>Id</t>
   </si>
@@ -211,6 +211,21 @@
   </si>
   <si>
     <t>p1_homepage</t>
+  </si>
+  <si>
+    <t>p2_dodawanie_edycja_imprezy</t>
+  </si>
+  <si>
+    <t>p3_wyszukanie_imprez</t>
+  </si>
+  <si>
+    <t>p4_usuniecie_imprezy</t>
+  </si>
+  <si>
+    <t>p5_wyszukanie_skladnikow</t>
+  </si>
+  <si>
+    <t>p6_usuniecie_skladnika</t>
   </si>
 </sst>
 </file>
@@ -569,8 +584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -633,7 +648,9 @@
       <c r="G2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="2"/>
+      <c r="H2" s="2" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
@@ -657,7 +674,9 @@
       <c r="G3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H3" s="2"/>
+      <c r="H3" s="2" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
@@ -681,7 +700,9 @@
       <c r="G4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="2"/>
+      <c r="H4" s="2" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
@@ -705,7 +726,9 @@
       <c r="G5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H5" s="2"/>
+      <c r="H5" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="6" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
@@ -729,7 +752,9 @@
       <c r="G6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H6" s="2"/>
+      <c r="H6" s="2" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
@@ -795,7 +820,9 @@
         <v>18</v>
       </c>
       <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
+      <c r="H9" s="2" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2">

</xml_diff>

<commit_message>
Poprawione nazwy prototypow, uspojnione historie
</commit_message>
<xml_diff>
--- a/historie.xlsx
+++ b/historie.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="88">
   <si>
     <t>Id</t>
   </si>
@@ -69,9 +69,6 @@
     <t>mieć możliwość tworzenia składników imprez turystycznych</t>
   </si>
   <si>
-    <t>Współdzielenie danych takich jak np. dojadzd autokarem, samolotem, all inclusive.</t>
-  </si>
-  <si>
     <t>zaktualizować ofertę</t>
   </si>
   <si>
@@ -96,12 +93,6 @@
     <t>Np. dodawanie kolejnych turnusów.</t>
   </si>
   <si>
-    <t>Dane to m.in. miejsce, opis, regulamin, zdjęcia.</t>
-  </si>
-  <si>
-    <t>Katalogi w postaci struktury drzewiastej.</t>
-  </si>
-  <si>
     <t>mieć możliwość edycji terminów imprez turystycznych</t>
   </si>
   <si>
@@ -210,22 +201,85 @@
     <t>mieć możliwość usunięcia państw, miast, hoteli ze słownika</t>
   </si>
   <si>
-    <t>p1_homepage</t>
-  </si>
-  <si>
-    <t>p2_dodawanie_edycja_imprezy</t>
-  </si>
-  <si>
-    <t>p3_wyszukanie_imprez</t>
-  </si>
-  <si>
-    <t>p4_usuniecie_imprezy</t>
-  </si>
-  <si>
     <t>p5_wyszukanie_skladnikow</t>
   </si>
   <si>
-    <t>p6_usuniecie_skladnika</t>
+    <t>p3_dodawanie_edycja_imprezy</t>
+  </si>
+  <si>
+    <t>p2_wyszukanie_imprez</t>
+  </si>
+  <si>
+    <t>p4_usuwanie_imprezy</t>
+  </si>
+  <si>
+    <t>p6_usuwanie_skladnika</t>
+  </si>
+  <si>
+    <t>p7_dodawanie_edycja_skladnika</t>
+  </si>
+  <si>
+    <t>p8_wyszukanie_katalogow</t>
+  </si>
+  <si>
+    <t>p9_dodawanie_edycja_katalogu</t>
+  </si>
+  <si>
+    <t>p10_usuwanie_katalogu</t>
+  </si>
+  <si>
+    <t>p11_wyszukanie_terminow</t>
+  </si>
+  <si>
+    <t>p12_dodawanie_terminu</t>
+  </si>
+  <si>
+    <t>p13_edycja_terminu</t>
+  </si>
+  <si>
+    <t>p14_usuwanie_terminow</t>
+  </si>
+  <si>
+    <t>p15_wyszukanie_w_slowniku</t>
+  </si>
+  <si>
+    <t>p16_dodawanie_edycja_miasta_w_slowniku p17_dodawanie_edycja_hotelu_w_slowniku p18_dodawanie_edycja_panstwa_w_slowniku</t>
+  </si>
+  <si>
+    <t>p19_usuwanie_w_slowniku</t>
+  </si>
+  <si>
+    <t>p1_homepage p23_wyszukanie_imprez_przez_klienta p24_podglad_imprezy_klient</t>
+  </si>
+  <si>
+    <t>p26_cennik_imprezy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p23_wyszukanie_imprez_przez_klienta </t>
+  </si>
+  <si>
+    <t>p27_platnosc_po_rezerwacji</t>
+  </si>
+  <si>
+    <t>p25_rezerwacja_imprezy</t>
+  </si>
+  <si>
+    <t>p28_rezygnacja</t>
+  </si>
+  <si>
+    <t>p20_wyszukanie_cennikow</t>
+  </si>
+  <si>
+    <t>p21_dodawanie_edycja_cenniku</t>
+  </si>
+  <si>
+    <t>p22_usuwanie_cennikow</t>
+  </si>
+  <si>
+    <t>Dane to nazwa, miejsce, opis, regulamin, zdjęcia, wyżywienie, zakwaterowanie, transport.</t>
+  </si>
+  <si>
+    <t>Dane to nazwa, miejsce, opis, wyżywienie, zakwaterowanie, transport.</t>
   </si>
 </sst>
 </file>
@@ -585,7 +639,7 @@
   <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -608,7 +662,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>2</v>
@@ -634,7 +688,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>8</v>
@@ -643,13 +697,13 @@
         <v>11</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>26</v>
+        <v>86</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -660,7 +714,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>8</v>
@@ -669,13 +723,13 @@
         <v>12</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>26</v>
+        <v>87</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -686,7 +740,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>8</v>
@@ -695,13 +749,13 @@
         <v>14</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>26</v>
+        <v>86</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -712,7 +766,7 @@
         <v>7</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>8</v>
@@ -721,13 +775,13 @@
         <v>13</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>26</v>
+        <v>86</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -738,7 +792,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>8</v>
@@ -749,11 +803,9 @@
       <c r="F6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>17</v>
-      </c>
+      <c r="G6" s="2"/>
       <c r="H6" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -764,19 +816,21 @@
         <v>7</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
+      <c r="H7" s="2" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
@@ -786,19 +840,21 @@
         <v>7</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
+      <c r="H8" s="2" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
@@ -808,20 +864,20 @@
         <v>7</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -832,21 +888,21 @@
         <v>7</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="H10" s="2"/>
+        <v>19</v>
+      </c>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
@@ -856,19 +912,21 @@
         <v>7</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
+      <c r="H11" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
@@ -878,19 +936,21 @@
         <v>7</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
+      <c r="H12" s="2" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
@@ -900,19 +960,21 @@
         <v>7</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
+      <c r="H13" s="2" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
@@ -922,21 +984,23 @@
         <v>7</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G14" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F14" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H14" s="2"/>
+      <c r="H14" s="2" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
@@ -946,19 +1010,21 @@
         <v>7</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
+      <c r="H15" s="2" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
@@ -968,19 +1034,21 @@
         <v>7</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
+      <c r="H16" s="2" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
@@ -990,19 +1058,21 @@
         <v>7</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
+      <c r="H17" s="2" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
@@ -1012,21 +1082,23 @@
         <v>7</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="H18" s="2"/>
+        <v>48</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
@@ -1036,19 +1108,21 @@
         <v>7</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
+      <c r="H19" s="2" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
@@ -1058,19 +1132,21 @@
         <v>7</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
+      <c r="H20" s="2" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
@@ -1080,21 +1156,23 @@
         <v>7</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-    </row>
-    <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="H21" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -1102,19 +1180,21 @@
         <v>7</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
+      <c r="H22" s="2" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
@@ -1124,21 +1204,23 @@
         <v>7</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-    </row>
-    <row r="24" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="H23" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -1146,19 +1228,21 @@
         <v>7</v>
       </c>
       <c r="C24" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D24" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>62</v>
-      </c>
       <c r="F24" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
+      <c r="H24" s="2" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
@@ -1168,19 +1252,21 @@
         <v>7</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
+      <c r="H25" s="2" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
@@ -1190,21 +1276,23 @@
         <v>7</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-    </row>
-    <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="H26" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -1212,20 +1300,20 @@
         <v>9</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G27" s="2"/>
       <c r="H27" s="2" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1236,19 +1324,21 @@
         <v>9</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
+      <c r="H28" s="2" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="29" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
@@ -1258,21 +1348,23 @@
         <v>9</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E29" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G29" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="F29" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H29" s="2"/>
+      <c r="H29" s="2" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
@@ -1282,21 +1374,23 @@
         <v>9</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="H30" s="2"/>
+        <v>46</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="31" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
@@ -1306,19 +1400,21 @@
         <v>9</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
+      <c r="H31" s="2" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
@@ -1328,19 +1424,21 @@
         <v>9</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
+      <c r="H32" s="2" t="s">
+        <v>82</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>